<commit_message>
Update specs add adtrr long version
</commit_message>
<xml_diff>
--- a/specifications/er_spec.xlsx
+++ b/specifications/er_spec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff.dickinson\Documents\GitHub\er-standards\specifications\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{153B52A6-064B-45D2-8920-39D4F4FDD671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC23F31-63F0-45AE-94E7-FA2435AD807E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Study" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Documents!$A$1:$C$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Methods!$A$1:$H$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ValueLevel!$A$1:$P$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$1:$P$300</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$1:$P$367</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">WhereClauses!$A$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2229" uniqueCount="716">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2137" uniqueCount="675">
   <si>
     <t>Attribute</t>
   </si>
@@ -1953,9 +1953,6 @@
     <t>Actual Treatment for Period 01 (N)</t>
   </si>
   <si>
-    <t>Actual Dose (mg)</t>
-  </si>
-  <si>
     <t>AVALC</t>
   </si>
   <si>
@@ -2061,154 +2058,34 @@
     <t>Treatment Emergent Analysis Flag</t>
   </si>
   <si>
-    <t>AOCCFL</t>
-  </si>
-  <si>
-    <t>1st Occurrence within Subject Flag</t>
-  </si>
-  <si>
     <t>Steady-State Area Under Curve</t>
   </si>
   <si>
     <t>Steady-State Maximum Concentration</t>
   </si>
   <si>
-    <t>Steady-State Average Concentration</t>
-  </si>
-  <si>
-    <t>Log Steady-State AUC</t>
-  </si>
-  <si>
-    <t>CMXSLOG</t>
-  </si>
-  <si>
-    <t>Log Steady-State Cmax</t>
-  </si>
-  <si>
-    <t>CAVGLOG</t>
-  </si>
-  <si>
-    <t>Log Steady-State Cavg</t>
-  </si>
-  <si>
-    <t>Standardized Steady-State AUC</t>
-  </si>
-  <si>
-    <t>CMXSSSTD</t>
-  </si>
-  <si>
-    <t>Standardized Steady-State Cmax</t>
-  </si>
-  <si>
-    <t>CAVGSTD</t>
-  </si>
-  <si>
-    <t>Standardized Steady-State Cavg</t>
-  </si>
-  <si>
-    <t>Normalized Steady-State AUC</t>
-  </si>
-  <si>
-    <t>CMAXSSN</t>
-  </si>
-  <si>
-    <t>Normalized Steady-State Cmax</t>
-  </si>
-  <si>
-    <t>CAVGSSN</t>
-  </si>
-  <si>
-    <t>Normalized Steady-State Cavg</t>
-  </si>
-  <si>
-    <t>Dose-Normalized Steady-State AUC</t>
-  </si>
-  <si>
-    <t>CMXSSDOS</t>
-  </si>
-  <si>
-    <t>Dose-Normalized Steady-State Cmax</t>
-  </si>
-  <si>
-    <t>CAVGDOS</t>
-  </si>
-  <si>
-    <t>Dose-Normalized Steady-State Cavg</t>
-  </si>
-  <si>
-    <t>Steady-State AUC Category</t>
-  </si>
-  <si>
-    <t>Steady-State AUC Category (N)</t>
-  </si>
-  <si>
-    <t>CMXSSCAT</t>
-  </si>
-  <si>
-    <t>Steady-State Cmax Category</t>
-  </si>
-  <si>
-    <t>CMXSCATN</t>
-  </si>
-  <si>
-    <t>Steady-State Cmax Category (N)</t>
-  </si>
-  <si>
     <t>Baseline Body Mass Index (kg/m2)</t>
   </si>
   <si>
-    <t>BSA</t>
-  </si>
-  <si>
-    <t>Body Surface Area (m2)</t>
-  </si>
-  <si>
     <t>Baseline Creatinine (mg/dL)</t>
   </si>
   <si>
     <t>Baseline eGFR (mL/min/1.73m2)</t>
   </si>
   <si>
-    <t>Baseline Alanine Aminotransferase (U/L)</t>
-  </si>
-  <si>
-    <t>Baseline Aspartate Aminotransferase (U/L)</t>
-  </si>
-  <si>
-    <t>ECOGBL</t>
-  </si>
-  <si>
-    <t>Baseline ECOG Performance Status</t>
-  </si>
-  <si>
-    <t>SMOKEBL</t>
-  </si>
-  <si>
-    <t>Baseline Smoking Status</t>
-  </si>
-  <si>
     <t>Analysis Flag 01 (Primary Analysis)</t>
   </si>
   <si>
     <t>Analysis Flag 02 (Event-Level Analysis)</t>
   </si>
   <si>
-    <t>ITTFL</t>
-  </si>
-  <si>
-    <t>Intent-to-Treat Population Flag</t>
-  </si>
-  <si>
-    <t>EFFFL</t>
-  </si>
-  <si>
-    <t>Efficacy Population Flag</t>
-  </si>
-  <si>
     <t>ADES</t>
   </si>
   <si>
     <t>Exposure Safety Analysis Data</t>
+  </si>
+  <si>
+    <t>Baseline Body Surface Area (m2)</t>
   </si>
 </sst>
 </file>
@@ -2832,9 +2709,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2988,10 +2865,10 @@
     </row>
     <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>715</v>
+        <v>673</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>392</v>
@@ -3051,13 +2928,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:P390"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:P367"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D368" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D303" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I394" sqref="I394"/>
+      <selection pane="bottomRight" activeCell="K314" sqref="K314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3130,7 +3008,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3153,7 +3031,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="3" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3176,7 +3054,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3199,7 +3077,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3222,7 +3100,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3245,7 +3123,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3268,7 +3146,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="8" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3291,7 +3169,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="9" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3314,7 +3192,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3340,7 +3218,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="11" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3366,7 +3244,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="12" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3389,7 +3267,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3409,7 +3287,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3438,7 +3316,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3464,7 +3342,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3490,7 +3368,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3516,7 +3394,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3542,7 +3420,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3568,7 +3446,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3594,7 +3472,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="21" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3620,7 +3498,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="22" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3643,7 +3521,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3666,7 +3544,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="24" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3689,7 +3567,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="25" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3712,7 +3590,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="26" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3735,7 +3613,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="27" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3758,7 +3636,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="28" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3781,7 +3659,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="29" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3804,7 +3682,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="30" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3830,7 +3708,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="31" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3856,7 +3734,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="32" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3876,7 +3754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3896,7 +3774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3922,7 +3800,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="35" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3948,7 +3826,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="36" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3971,7 +3849,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="37" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3994,7 +3872,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="38" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4017,7 +3895,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="39" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4037,7 +3915,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4060,7 +3938,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="41" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4083,7 +3961,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="42" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4103,7 +3981,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4129,7 +4007,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="44" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4149,7 +4027,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="45" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4169,7 +4047,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="46" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4189,7 +4067,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="47" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4209,7 +4087,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="48" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4232,7 +4110,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="49" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4255,7 +4133,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="50" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4281,7 +4159,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="51" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4304,7 +4182,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="52" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4327,7 +4205,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="53" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4350,7 +4228,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="54" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4370,7 +4248,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4390,7 +4268,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4410,7 +4288,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4430,7 +4308,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4450,7 +4328,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4470,7 +4348,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4490,7 +4368,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4510,7 +4388,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4530,7 +4408,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4550,7 +4428,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4570,7 +4448,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="65" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4593,7 +4471,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="66" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4616,7 +4494,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="67" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4639,7 +4517,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="68" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4662,7 +4540,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="69" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4685,7 +4563,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="70" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4708,7 +4586,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="71" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4728,7 +4606,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="72" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4748,7 +4626,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4768,7 +4646,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4788,7 +4666,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="75" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4808,7 +4686,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="76" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -4831,7 +4709,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="77" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -4854,7 +4732,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="78" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -4874,7 +4752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -4897,7 +4775,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="80" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -4917,7 +4795,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -4937,7 +4815,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="82" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -4957,7 +4835,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="83" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -4977,7 +4855,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="84" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -4997,7 +4875,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -5017,7 +4895,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -5037,7 +4915,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -5057,7 +4935,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="88" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -5077,7 +4955,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="89" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -5097,7 +4975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -5117,7 +4995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -5137,7 +5015,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="92" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -5157,7 +5035,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="93" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -5177,7 +5055,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="94" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -5197,7 +5075,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="95" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -5217,7 +5095,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="96" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -5237,7 +5115,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="97" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -5257,7 +5135,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="98" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -5277,7 +5155,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="99" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -5297,7 +5175,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="100" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -5317,7 +5195,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="101" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -5337,7 +5215,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="102" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -5357,7 +5235,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="103" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -5377,7 +5255,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="104" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -5397,7 +5275,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="105" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -5417,7 +5295,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="106" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -5437,7 +5315,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="107" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -5457,7 +5335,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="108" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -5480,7 +5358,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="109" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -5503,7 +5381,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="110" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -5526,7 +5404,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="111" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -5549,7 +5427,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="112" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -5572,7 +5450,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="113" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -5595,7 +5473,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="114" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -5615,7 +5493,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="115" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -5635,7 +5513,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="116" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -5655,7 +5533,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="117" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -5675,7 +5553,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="118" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -5695,7 +5573,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="119" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -5715,7 +5593,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="120" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -5735,7 +5613,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="121" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -5755,7 +5633,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="122" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -5775,7 +5653,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="123" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
@@ -5795,7 +5673,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="27">
         <v>1</v>
       </c>
@@ -5824,7 +5702,7 @@
       <c r="O124" s="10"/>
       <c r="P124" s="10"/>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="27">
         <v>2</v>
       </c>
@@ -5853,7 +5731,7 @@
       <c r="O125" s="10"/>
       <c r="P125" s="10"/>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="27">
         <v>3</v>
       </c>
@@ -5882,7 +5760,7 @@
       <c r="O126" s="10"/>
       <c r="P126" s="10"/>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="27">
         <v>4</v>
       </c>
@@ -5913,7 +5791,7 @@
       <c r="O127" s="10"/>
       <c r="P127" s="10"/>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="27">
         <v>5</v>
       </c>
@@ -5942,7 +5820,7 @@
       <c r="O128" s="10"/>
       <c r="P128" s="10"/>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="27">
         <v>6</v>
       </c>
@@ -5973,7 +5851,7 @@
       <c r="O129" s="10"/>
       <c r="P129" s="10"/>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="27">
         <v>7</v>
       </c>
@@ -6004,7 +5882,7 @@
       <c r="O130" s="10"/>
       <c r="P130" s="10"/>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="27">
         <v>8</v>
       </c>
@@ -6033,7 +5911,7 @@
       <c r="O131" s="10"/>
       <c r="P131" s="10"/>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="27">
         <v>9</v>
       </c>
@@ -6062,7 +5940,7 @@
       <c r="O132" s="10"/>
       <c r="P132" s="10"/>
     </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="27">
         <v>10</v>
       </c>
@@ -6091,7 +5969,7 @@
       <c r="O133" s="10"/>
       <c r="P133" s="10"/>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="27">
         <v>11</v>
       </c>
@@ -6120,7 +5998,7 @@
       <c r="O134" s="10"/>
       <c r="P134" s="10"/>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="27">
         <v>12</v>
       </c>
@@ -6149,7 +6027,7 @@
       <c r="O135" s="10"/>
       <c r="P135" s="10"/>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="27">
         <v>13</v>
       </c>
@@ -6178,7 +6056,7 @@
       <c r="O136" s="10"/>
       <c r="P136" s="10"/>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="27">
         <v>14</v>
       </c>
@@ -6207,7 +6085,7 @@
       <c r="O137" s="10"/>
       <c r="P137" s="10"/>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="27">
         <v>15</v>
       </c>
@@ -6236,7 +6114,7 @@
       <c r="O138" s="10"/>
       <c r="P138" s="10"/>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="27">
         <v>16</v>
       </c>
@@ -6265,7 +6143,7 @@
       <c r="O139" s="10"/>
       <c r="P139" s="10"/>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="27">
         <v>17</v>
       </c>
@@ -6294,7 +6172,7 @@
       <c r="O140" s="10"/>
       <c r="P140" s="10"/>
     </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="27">
         <v>18</v>
       </c>
@@ -6323,7 +6201,7 @@
       <c r="O141" s="10"/>
       <c r="P141" s="10"/>
     </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="27">
         <v>19</v>
       </c>
@@ -6352,7 +6230,7 @@
       <c r="O142" s="10"/>
       <c r="P142" s="10"/>
     </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="27">
         <v>20</v>
       </c>
@@ -6381,7 +6259,7 @@
       <c r="O143" s="10"/>
       <c r="P143" s="10"/>
     </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="27">
         <v>21</v>
       </c>
@@ -6412,7 +6290,7 @@
       <c r="O144" s="10"/>
       <c r="P144" s="10"/>
     </row>
-    <row r="145" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="27">
         <v>22</v>
       </c>
@@ -6443,7 +6321,7 @@
       <c r="O145" s="10"/>
       <c r="P145" s="10"/>
     </row>
-    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="27">
         <v>25</v>
       </c>
@@ -6472,7 +6350,7 @@
       <c r="O146" s="10"/>
       <c r="P146" s="10"/>
     </row>
-    <row r="147" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="27">
         <v>26</v>
       </c>
@@ -6501,7 +6379,7 @@
       <c r="O147" s="10"/>
       <c r="P147" s="10"/>
     </row>
-    <row r="148" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="27">
         <v>27</v>
       </c>
@@ -6532,7 +6410,7 @@
       <c r="O148" s="10"/>
       <c r="P148" s="10"/>
     </row>
-    <row r="149" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="27">
         <v>28</v>
       </c>
@@ -6561,7 +6439,7 @@
       <c r="O149" s="10"/>
       <c r="P149" s="10"/>
     </row>
-    <row r="150" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="27">
         <v>29</v>
       </c>
@@ -6590,7 +6468,7 @@
       <c r="O150" s="10"/>
       <c r="P150" s="10"/>
     </row>
-    <row r="151" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="27">
         <v>30</v>
       </c>
@@ -6619,7 +6497,7 @@
       <c r="O151" s="10"/>
       <c r="P151" s="10"/>
     </row>
-    <row r="152" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="27">
         <v>31</v>
       </c>
@@ -6648,7 +6526,7 @@
       <c r="O152" s="10"/>
       <c r="P152" s="10"/>
     </row>
-    <row r="153" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="27">
         <v>32</v>
       </c>
@@ -6677,7 +6555,7 @@
       <c r="O153" s="10"/>
       <c r="P153" s="10"/>
     </row>
-    <row r="154" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="27">
         <v>33</v>
       </c>
@@ -6706,7 +6584,7 @@
       <c r="O154" s="10"/>
       <c r="P154" s="10"/>
     </row>
-    <row r="155" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="27">
         <v>36</v>
       </c>
@@ -6726,7 +6604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="27">
         <v>37</v>
       </c>
@@ -6746,7 +6624,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="157" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="27">
         <v>40</v>
       </c>
@@ -6766,7 +6644,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="158" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="27">
         <v>41</v>
       </c>
@@ -6786,7 +6664,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="159" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="27">
         <v>45</v>
       </c>
@@ -6806,7 +6684,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="160" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="27">
         <v>46</v>
       </c>
@@ -6826,7 +6704,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="27">
         <v>47</v>
       </c>
@@ -6846,7 +6724,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="27">
         <v>48</v>
       </c>
@@ -6866,7 +6744,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="27">
         <v>49</v>
       </c>
@@ -6889,7 +6767,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="27">
         <v>50</v>
       </c>
@@ -6909,7 +6787,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="27">
         <v>51</v>
       </c>
@@ -6932,7 +6810,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="27">
         <v>54</v>
       </c>
@@ -6955,7 +6833,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="27">
         <v>55</v>
       </c>
@@ -6978,7 +6856,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="27">
         <v>56</v>
       </c>
@@ -6998,7 +6876,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="27">
         <v>58</v>
       </c>
@@ -7018,7 +6896,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="27">
         <v>59</v>
       </c>
@@ -7038,7 +6916,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="27">
         <v>60</v>
       </c>
@@ -7058,7 +6936,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="27">
         <v>61</v>
       </c>
@@ -7078,7 +6956,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="27">
         <v>62</v>
       </c>
@@ -7098,7 +6976,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="27">
         <v>64</v>
       </c>
@@ -7121,7 +6999,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="27">
         <v>65</v>
       </c>
@@ -7144,7 +7022,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="27">
         <v>66</v>
       </c>
@@ -7167,7 +7045,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="27">
         <v>67</v>
       </c>
@@ -7190,7 +7068,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="27">
         <v>70</v>
       </c>
@@ -7213,7 +7091,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="27">
         <v>71</v>
       </c>
@@ -7236,7 +7114,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="27">
         <v>72</v>
       </c>
@@ -7256,7 +7134,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="27">
         <v>73</v>
       </c>
@@ -7276,7 +7154,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="27">
         <v>74</v>
       </c>
@@ -7299,7 +7177,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="27">
         <v>75</v>
       </c>
@@ -7322,7 +7200,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="27">
         <v>76</v>
       </c>
@@ -7345,7 +7223,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="27">
         <v>77</v>
       </c>
@@ -7365,7 +7243,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="27">
         <v>78</v>
       </c>
@@ -7385,7 +7263,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="27">
         <v>79</v>
       </c>
@@ -7405,7 +7283,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="27">
         <v>80</v>
       </c>
@@ -7425,7 +7303,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="27">
         <v>81</v>
       </c>
@@ -7445,7 +7323,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="27">
         <v>82</v>
       </c>
@@ -7465,7 +7343,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>1</v>
       </c>
@@ -7488,7 +7366,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>2</v>
       </c>
@@ -7511,7 +7389,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>3</v>
       </c>
@@ -7534,7 +7412,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>4</v>
       </c>
@@ -7557,7 +7435,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="195" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>5</v>
       </c>
@@ -7580,7 +7458,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="196" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>6</v>
       </c>
@@ -7603,7 +7481,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>7</v>
       </c>
@@ -7626,7 +7504,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>8</v>
       </c>
@@ -7649,7 +7527,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>9</v>
       </c>
@@ -7672,7 +7550,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="200" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>10</v>
       </c>
@@ -7695,7 +7573,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="201" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>11</v>
       </c>
@@ -7718,7 +7596,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>12</v>
       </c>
@@ -7741,7 +7619,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>13</v>
       </c>
@@ -7764,7 +7642,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="204" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>14</v>
       </c>
@@ -7787,7 +7665,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>15</v>
       </c>
@@ -7810,7 +7688,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="206" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>16</v>
       </c>
@@ -7833,7 +7711,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>17</v>
       </c>
@@ -7856,7 +7734,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>18</v>
       </c>
@@ -7879,7 +7757,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>19</v>
       </c>
@@ -7902,7 +7780,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>20</v>
       </c>
@@ -7925,7 +7803,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>21</v>
       </c>
@@ -7948,7 +7826,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>22</v>
       </c>
@@ -7971,7 +7849,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>23</v>
       </c>
@@ -7994,7 +7872,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>24</v>
       </c>
@@ -8017,7 +7895,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>25</v>
       </c>
@@ -8040,7 +7918,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>26</v>
       </c>
@@ -8063,7 +7941,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>27</v>
       </c>
@@ -8086,7 +7964,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>28</v>
       </c>
@@ -8109,7 +7987,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>29</v>
       </c>
@@ -8132,7 +8010,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>30</v>
       </c>
@@ -8155,7 +8033,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="221" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>31</v>
       </c>
@@ -8178,7 +8056,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>32</v>
       </c>
@@ -8201,7 +8079,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>33</v>
       </c>
@@ -8224,7 +8102,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>34</v>
       </c>
@@ -8247,7 +8125,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>35</v>
       </c>
@@ -8270,7 +8148,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>36</v>
       </c>
@@ -8293,7 +8171,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>37</v>
       </c>
@@ -8316,7 +8194,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>38</v>
       </c>
@@ -8339,7 +8217,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>39</v>
       </c>
@@ -8362,7 +8240,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>40</v>
       </c>
@@ -8385,7 +8263,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="231" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>41</v>
       </c>
@@ -8408,7 +8286,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="232" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>42</v>
       </c>
@@ -8431,7 +8309,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="233" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>43</v>
       </c>
@@ -8454,7 +8332,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>44</v>
       </c>
@@ -8477,7 +8355,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>45</v>
       </c>
@@ -8500,7 +8378,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="236" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>46</v>
       </c>
@@ -8520,7 +8398,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="237" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>47</v>
       </c>
@@ -8540,7 +8418,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>48</v>
       </c>
@@ -8560,7 +8438,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>49</v>
       </c>
@@ -8580,7 +8458,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>50</v>
       </c>
@@ -8600,7 +8478,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>51</v>
       </c>
@@ -8620,7 +8498,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>52</v>
       </c>
@@ -8640,7 +8518,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>53</v>
       </c>
@@ -8660,7 +8538,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>54</v>
       </c>
@@ -8680,7 +8558,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>55</v>
       </c>
@@ -8700,7 +8578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>56</v>
       </c>
@@ -8720,7 +8598,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>57</v>
       </c>
@@ -8740,7 +8618,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>58</v>
       </c>
@@ -8760,7 +8638,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>12</v>
       </c>
@@ -8780,7 +8658,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>13</v>
       </c>
@@ -8800,7 +8678,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>14</v>
       </c>
@@ -8820,7 +8698,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>15</v>
       </c>
@@ -8843,7 +8721,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>16</v>
       </c>
@@ -8866,7 +8744,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>17</v>
       </c>
@@ -8886,7 +8764,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>18</v>
       </c>
@@ -8906,7 +8784,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>19</v>
       </c>
@@ -8926,7 +8804,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>20</v>
       </c>
@@ -8946,7 +8824,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>21</v>
       </c>
@@ -8966,7 +8844,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>22</v>
       </c>
@@ -8986,7 +8864,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>23</v>
       </c>
@@ -9006,7 +8884,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>24</v>
       </c>
@@ -9026,7 +8904,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>25</v>
       </c>
@@ -9049,7 +8927,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>26</v>
       </c>
@@ -9072,7 +8950,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>28</v>
       </c>
@@ -9092,7 +8970,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>29</v>
       </c>
@@ -9112,7 +8990,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>30</v>
       </c>
@@ -9132,7 +9010,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>31</v>
       </c>
@@ -9152,7 +9030,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>32</v>
       </c>
@@ -9172,7 +9050,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>33</v>
       </c>
@@ -9192,7 +9070,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>34</v>
       </c>
@@ -9212,7 +9090,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>35</v>
       </c>
@@ -9232,7 +9110,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>40</v>
       </c>
@@ -9252,7 +9130,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>41</v>
       </c>
@@ -9272,7 +9150,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>42</v>
       </c>
@@ -9292,7 +9170,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>43</v>
       </c>
@@ -9312,7 +9190,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>44</v>
       </c>
@@ -9332,7 +9210,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>45</v>
       </c>
@@ -9352,7 +9230,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>46</v>
       </c>
@@ -9372,7 +9250,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>47</v>
       </c>
@@ -9392,7 +9270,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>48</v>
       </c>
@@ -9412,7 +9290,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>49</v>
       </c>
@@ -9432,7 +9310,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>50</v>
       </c>
@@ -9452,7 +9330,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>51</v>
       </c>
@@ -9472,7 +9350,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>52</v>
       </c>
@@ -9492,7 +9370,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>53</v>
       </c>
@@ -9512,7 +9390,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>54</v>
       </c>
@@ -9532,7 +9410,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>55</v>
       </c>
@@ -9552,7 +9430,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>56</v>
       </c>
@@ -9572,7 +9450,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>57</v>
       </c>
@@ -9592,7 +9470,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>58</v>
       </c>
@@ -9612,7 +9490,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>59</v>
       </c>
@@ -9632,7 +9510,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>60</v>
       </c>
@@ -9652,7 +9530,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>61</v>
       </c>
@@ -9672,7 +9550,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>62</v>
       </c>
@@ -9692,7 +9570,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>63</v>
       </c>
@@ -9712,7 +9590,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>64</v>
       </c>
@@ -9732,7 +9610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>65</v>
       </c>
@@ -9752,7 +9630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>66</v>
       </c>
@@ -9772,7 +9650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>67</v>
       </c>
@@ -9792,7 +9670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>68</v>
       </c>
@@ -9817,7 +9695,7 @@
         <v>1</v>
       </c>
       <c r="B301" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C301" t="s">
         <v>51</v>
@@ -9837,7 +9715,7 @@
         <v>2</v>
       </c>
       <c r="B302" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C302" t="s">
         <v>402</v>
@@ -9855,7 +9733,7 @@
         <v>3</v>
       </c>
       <c r="B303" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C303" t="s">
         <v>52</v>
@@ -9875,7 +9753,7 @@
         <v>4</v>
       </c>
       <c r="B304" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C304" t="s">
         <v>411</v>
@@ -9893,7 +9771,7 @@
         <v>5</v>
       </c>
       <c r="B305" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C305" t="s">
         <v>55</v>
@@ -9913,7 +9791,7 @@
         <v>6</v>
       </c>
       <c r="B306" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C306" t="s">
         <v>413</v>
@@ -9931,7 +9809,7 @@
         <v>7</v>
       </c>
       <c r="B307" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C307" t="s">
         <v>64</v>
@@ -9951,7 +9829,7 @@
         <v>8</v>
       </c>
       <c r="B308" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C308" t="s">
         <v>415</v>
@@ -9969,7 +9847,7 @@
         <v>9</v>
       </c>
       <c r="B309" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C309" t="s">
         <v>384</v>
@@ -9987,7 +9865,7 @@
         <v>10</v>
       </c>
       <c r="B310" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C310" t="s">
         <v>71</v>
@@ -10007,7 +9885,7 @@
         <v>11</v>
       </c>
       <c r="B311" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C311" t="s">
         <v>518</v>
@@ -10025,7 +9903,7 @@
         <v>12</v>
       </c>
       <c r="B312" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C312" t="s">
         <v>70</v>
@@ -10045,7 +9923,7 @@
         <v>13</v>
       </c>
       <c r="B313" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C313" t="s">
         <v>206</v>
@@ -10065,7 +9943,7 @@
         <v>14</v>
       </c>
       <c r="B314" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C314" t="s">
         <v>626</v>
@@ -10083,7 +9961,7 @@
         <v>15</v>
       </c>
       <c r="B315" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C315" t="s">
         <v>208</v>
@@ -10103,7 +9981,7 @@
         <v>16</v>
       </c>
       <c r="B316" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C316" t="s">
         <v>628</v>
@@ -10118,318 +9996,320 @@
     </row>
     <row r="317" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A317">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B317" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C317" t="s">
-        <v>520</v>
+        <v>65</v>
       </c>
       <c r="D317" t="s">
-        <v>630</v>
+        <v>98</v>
       </c>
       <c r="E317" t="s">
-        <v>544</v>
+        <v>528</v>
       </c>
       <c r="F317"/>
     </row>
     <row r="318" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A318">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B318" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C318" t="s">
-        <v>65</v>
+        <v>195</v>
       </c>
       <c r="D318" t="s">
-        <v>98</v>
+        <v>196</v>
       </c>
       <c r="E318" t="s">
-        <v>528</v>
-      </c>
-      <c r="F318"/>
+        <v>108</v>
+      </c>
+      <c r="F318">
+        <v>200</v>
+      </c>
     </row>
     <row r="319" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A319">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B319" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C319" t="s">
-        <v>195</v>
+        <v>575</v>
       </c>
       <c r="D319" t="s">
-        <v>196</v>
+        <v>576</v>
       </c>
       <c r="E319" t="s">
-        <v>108</v>
-      </c>
-      <c r="F319">
-        <v>200</v>
-      </c>
+        <v>528</v>
+      </c>
+      <c r="F319"/>
     </row>
     <row r="320" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A320">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B320" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C320" t="s">
-        <v>575</v>
+        <v>67</v>
       </c>
       <c r="D320" t="s">
-        <v>576</v>
+        <v>100</v>
       </c>
       <c r="E320" t="s">
-        <v>528</v>
-      </c>
-      <c r="F320"/>
+        <v>108</v>
+      </c>
+      <c r="F320">
+        <v>200</v>
+      </c>
     </row>
     <row r="321" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A321">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B321" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C321" t="s">
-        <v>67</v>
+        <v>480</v>
       </c>
       <c r="D321" t="s">
-        <v>100</v>
+        <v>481</v>
       </c>
       <c r="E321" t="s">
-        <v>108</v>
-      </c>
-      <c r="F321">
-        <v>200</v>
-      </c>
+        <v>528</v>
+      </c>
+      <c r="F321"/>
     </row>
     <row r="322" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A322">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B322" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C322" t="s">
-        <v>480</v>
+        <v>68</v>
       </c>
       <c r="D322" t="s">
-        <v>481</v>
+        <v>101</v>
       </c>
       <c r="E322" t="s">
-        <v>528</v>
-      </c>
-      <c r="F322"/>
+        <v>108</v>
+      </c>
+      <c r="F322">
+        <v>200</v>
+      </c>
     </row>
     <row r="323" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A323">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B323" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C323" t="s">
-        <v>68</v>
+        <v>482</v>
       </c>
       <c r="D323" t="s">
-        <v>101</v>
+        <v>483</v>
       </c>
       <c r="E323" t="s">
-        <v>108</v>
-      </c>
-      <c r="F323">
-        <v>200</v>
-      </c>
+        <v>528</v>
+      </c>
+      <c r="F323"/>
     </row>
     <row r="324" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A324">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B324" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C324" t="s">
-        <v>482</v>
+        <v>69</v>
       </c>
       <c r="D324" t="s">
-        <v>483</v>
+        <v>531</v>
       </c>
       <c r="E324" t="s">
-        <v>528</v>
-      </c>
-      <c r="F324"/>
+        <v>108</v>
+      </c>
+      <c r="F324">
+        <v>200</v>
+      </c>
     </row>
     <row r="325" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A325">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B325" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C325" t="s">
-        <v>69</v>
+        <v>532</v>
       </c>
       <c r="D325" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="E325" t="s">
-        <v>108</v>
-      </c>
-      <c r="F325">
-        <v>200</v>
-      </c>
+        <v>528</v>
+      </c>
+      <c r="F325"/>
     </row>
     <row r="326" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A326">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B326" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C326" t="s">
-        <v>532</v>
+        <v>256</v>
       </c>
       <c r="D326" t="s">
-        <v>533</v>
+        <v>257</v>
       </c>
       <c r="E326" t="s">
-        <v>528</v>
-      </c>
-      <c r="F326"/>
+        <v>108</v>
+      </c>
+      <c r="F326">
+        <v>8</v>
+      </c>
     </row>
     <row r="327" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A327">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B327" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C327" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D327" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E327" t="s">
         <v>108</v>
       </c>
       <c r="F327">
-        <v>8</v>
+        <v>200</v>
       </c>
     </row>
     <row r="328" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A328">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B328" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C328" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D328" t="s">
-        <v>253</v>
+        <v>578</v>
       </c>
       <c r="E328" t="s">
-        <v>108</v>
-      </c>
-      <c r="F328">
-        <v>200</v>
-      </c>
+        <v>528</v>
+      </c>
+      <c r="F328"/>
     </row>
     <row r="329" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A329">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B329" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C329" t="s">
-        <v>254</v>
+        <v>312</v>
       </c>
       <c r="D329" t="s">
-        <v>578</v>
+        <v>313</v>
       </c>
       <c r="E329" t="s">
-        <v>528</v>
+        <v>544</v>
       </c>
       <c r="F329"/>
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A330">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B330" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C330" t="s">
-        <v>312</v>
+        <v>630</v>
       </c>
       <c r="D330" t="s">
-        <v>313</v>
+        <v>631</v>
       </c>
       <c r="E330" t="s">
-        <v>544</v>
-      </c>
-      <c r="F330"/>
+        <v>108</v>
+      </c>
+      <c r="F330">
+        <v>200</v>
+      </c>
     </row>
     <row r="331" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A331">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B331" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C331" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="D331" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="E331" t="s">
-        <v>108</v>
-      </c>
-      <c r="F331">
-        <v>200</v>
-      </c>
+        <v>528</v>
+      </c>
+      <c r="F331"/>
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A332">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B332" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C332" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="D332" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="E332" t="s">
-        <v>528</v>
-      </c>
-      <c r="F332"/>
+        <v>108</v>
+      </c>
+      <c r="F332">
+        <v>200</v>
+      </c>
     </row>
     <row r="333" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A333">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B333" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C333" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="D333" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="E333" t="s">
         <v>108</v>
@@ -10440,16 +10320,16 @@
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A334">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B334" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C334" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="D334" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="E334" t="s">
         <v>108</v>
@@ -10460,16 +10340,16 @@
     </row>
     <row r="335" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A335">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B335" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C335" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="D335" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="E335" t="s">
         <v>108</v>
@@ -10480,112 +10360,112 @@
     </row>
     <row r="336" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A336">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B336" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C336" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="D336" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="E336" t="s">
-        <v>108</v>
-      </c>
-      <c r="F336">
-        <v>200</v>
-      </c>
+        <v>528</v>
+      </c>
+      <c r="F336"/>
     </row>
     <row r="337" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A337">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B337" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C337" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="D337" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="E337" t="s">
-        <v>528</v>
-      </c>
-      <c r="F337"/>
+        <v>108</v>
+      </c>
+      <c r="F337">
+        <v>200</v>
+      </c>
     </row>
     <row r="338" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A338">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B338" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C338" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="D338" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="E338" t="s">
-        <v>108</v>
-      </c>
-      <c r="F338">
-        <v>200</v>
-      </c>
+        <v>528</v>
+      </c>
+      <c r="F338"/>
     </row>
     <row r="339" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A339">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B339" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C339" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="D339" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="E339" t="s">
-        <v>528</v>
-      </c>
-      <c r="F339"/>
+        <v>108</v>
+      </c>
+      <c r="F339">
+        <v>1</v>
+      </c>
     </row>
     <row r="340" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A340">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B340" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C340" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="D340" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="E340" t="s">
         <v>108</v>
       </c>
       <c r="F340">
-        <v>1</v>
+        <v>200</v>
       </c>
     </row>
     <row r="341" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A341">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B341" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C341" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="D341" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="E341" t="s">
         <v>108</v>
@@ -10596,90 +10476,88 @@
     </row>
     <row r="342" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A342">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B342" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C342" t="s">
-        <v>653</v>
+        <v>360</v>
       </c>
       <c r="D342" t="s">
+        <v>361</v>
+      </c>
+      <c r="E342" t="s">
         <v>654</v>
       </c>
-      <c r="E342" t="s">
-        <v>108</v>
-      </c>
-      <c r="F342">
-        <v>200</v>
-      </c>
+      <c r="F342"/>
     </row>
     <row r="343" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A343">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B343" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C343" t="s">
-        <v>360</v>
+        <v>655</v>
       </c>
       <c r="D343" t="s">
-        <v>361</v>
+        <v>656</v>
       </c>
       <c r="E343" t="s">
-        <v>655</v>
+        <v>528</v>
       </c>
       <c r="F343"/>
     </row>
     <row r="344" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A344">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B344" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C344" t="s">
-        <v>656</v>
+        <v>366</v>
       </c>
       <c r="D344" t="s">
-        <v>657</v>
+        <v>367</v>
       </c>
       <c r="E344" t="s">
-        <v>528</v>
+        <v>654</v>
       </c>
       <c r="F344"/>
     </row>
     <row r="345" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A345">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B345" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C345" t="s">
-        <v>366</v>
+        <v>657</v>
       </c>
       <c r="D345" t="s">
-        <v>367</v>
+        <v>658</v>
       </c>
       <c r="E345" t="s">
-        <v>655</v>
+        <v>528</v>
       </c>
       <c r="F345"/>
     </row>
     <row r="346" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A346">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B346" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C346" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="D346" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="E346" t="s">
         <v>528</v>
@@ -10688,94 +10566,92 @@
     </row>
     <row r="347" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A347">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B347" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C347" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="D347" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="E347" t="s">
-        <v>528</v>
-      </c>
-      <c r="F347"/>
+        <v>108</v>
+      </c>
+      <c r="F347">
+        <v>200</v>
+      </c>
     </row>
     <row r="348" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A348">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B348" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C348" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="D348" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="E348" t="s">
         <v>108</v>
       </c>
       <c r="F348">
-        <v>200</v>
+        <v>1</v>
       </c>
     </row>
     <row r="349" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A349">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B349" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C349" t="s">
-        <v>664</v>
+        <v>593</v>
       </c>
       <c r="D349" t="s">
         <v>665</v>
       </c>
       <c r="E349" t="s">
-        <v>108</v>
-      </c>
-      <c r="F349">
-        <v>1</v>
-      </c>
+        <v>544</v>
+      </c>
+      <c r="F349"/>
     </row>
     <row r="350" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A350">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B350" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C350" t="s">
+        <v>609</v>
+      </c>
+      <c r="D350" t="s">
         <v>666</v>
       </c>
-      <c r="D350" t="s">
-        <v>667</v>
-      </c>
       <c r="E350" t="s">
-        <v>108</v>
-      </c>
-      <c r="F350">
-        <v>1</v>
-      </c>
+        <v>544</v>
+      </c>
+      <c r="F350"/>
     </row>
     <row r="351" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A351">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="B351" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C351" t="s">
-        <v>593</v>
+        <v>372</v>
       </c>
       <c r="D351" t="s">
-        <v>668</v>
+        <v>560</v>
       </c>
       <c r="E351" t="s">
         <v>544</v>
@@ -10784,16 +10660,16 @@
     </row>
     <row r="352" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A352">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="B352" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C352" t="s">
-        <v>609</v>
+        <v>374</v>
       </c>
       <c r="D352" t="s">
-        <v>669</v>
+        <v>561</v>
       </c>
       <c r="E352" t="s">
         <v>544</v>
@@ -10802,16 +10678,16 @@
     </row>
     <row r="353" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A353">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="B353" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C353" t="s">
-        <v>611</v>
+        <v>376</v>
       </c>
       <c r="D353" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="E353" t="s">
         <v>544</v>
@@ -10820,16 +10696,16 @@
     </row>
     <row r="354" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A354">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="B354" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C354" t="s">
-        <v>594</v>
+        <v>477</v>
       </c>
       <c r="D354" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="E354" t="s">
         <v>544</v>
@@ -10838,16 +10714,16 @@
     </row>
     <row r="355" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A355">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="B355" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C355" t="s">
-        <v>672</v>
+        <v>494</v>
       </c>
       <c r="D355" t="s">
-        <v>673</v>
+        <v>668</v>
       </c>
       <c r="E355" t="s">
         <v>544</v>
@@ -10856,16 +10732,16 @@
     </row>
     <row r="356" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A356">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="B356" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C356" t="s">
-        <v>674</v>
+        <v>496</v>
       </c>
       <c r="D356" t="s">
-        <v>675</v>
+        <v>565</v>
       </c>
       <c r="E356" t="s">
         <v>544</v>
@@ -10874,16 +10750,16 @@
     </row>
     <row r="357" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A357">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="B357" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C357" t="s">
-        <v>596</v>
+        <v>498</v>
       </c>
       <c r="D357" t="s">
-        <v>676</v>
+        <v>669</v>
       </c>
       <c r="E357" t="s">
         <v>544</v>
@@ -10892,16 +10768,16 @@
     </row>
     <row r="358" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A358">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="B358" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C358" t="s">
-        <v>677</v>
-      </c>
-      <c r="D358" t="s">
-        <v>678</v>
+        <v>504</v>
+      </c>
+      <c r="D358" s="15" t="s">
+        <v>567</v>
       </c>
       <c r="E358" t="s">
         <v>544</v>
@@ -10910,16 +10786,16 @@
     </row>
     <row r="359" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A359">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="B359" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C359" t="s">
-        <v>679</v>
-      </c>
-      <c r="D359" t="s">
-        <v>680</v>
+        <v>502</v>
+      </c>
+      <c r="D359" s="15" t="s">
+        <v>568</v>
       </c>
       <c r="E359" t="s">
         <v>544</v>
@@ -10928,16 +10804,16 @@
     </row>
     <row r="360" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A360">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="B360" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C360" t="s">
-        <v>598</v>
+        <v>500</v>
       </c>
       <c r="D360" t="s">
-        <v>681</v>
+        <v>569</v>
       </c>
       <c r="E360" t="s">
         <v>544</v>
@@ -10946,16 +10822,16 @@
     </row>
     <row r="361" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A361">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="B361" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C361" t="s">
-        <v>682</v>
+        <v>617</v>
       </c>
       <c r="D361" t="s">
-        <v>683</v>
+        <v>618</v>
       </c>
       <c r="E361" t="s">
         <v>544</v>
@@ -10964,544 +10840,126 @@
     </row>
     <row r="362" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A362">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="B362" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C362" t="s">
-        <v>684</v>
+        <v>219</v>
       </c>
       <c r="D362" t="s">
-        <v>685</v>
+        <v>220</v>
       </c>
       <c r="E362" t="s">
-        <v>544</v>
+        <v>654</v>
       </c>
       <c r="F362"/>
     </row>
     <row r="363" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A363">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="B363" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C363" t="s">
-        <v>600</v>
+        <v>221</v>
       </c>
       <c r="D363" t="s">
-        <v>686</v>
+        <v>222</v>
       </c>
       <c r="E363" t="s">
-        <v>544</v>
+        <v>654</v>
       </c>
       <c r="F363"/>
     </row>
     <row r="364" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A364">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="B364" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C364" t="s">
-        <v>687</v>
+        <v>230</v>
       </c>
       <c r="D364" t="s">
-        <v>688</v>
+        <v>577</v>
       </c>
       <c r="E364" t="s">
-        <v>544</v>
+        <v>528</v>
       </c>
       <c r="F364"/>
     </row>
     <row r="365" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A365">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="B365" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C365" t="s">
-        <v>689</v>
+        <v>328</v>
       </c>
       <c r="D365" t="s">
-        <v>690</v>
+        <v>670</v>
       </c>
       <c r="E365" t="s">
-        <v>544</v>
-      </c>
-      <c r="F365"/>
+        <v>108</v>
+      </c>
+      <c r="F365">
+        <v>1</v>
+      </c>
     </row>
     <row r="366" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A366">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="B366" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C366" t="s">
-        <v>601</v>
+        <v>326</v>
       </c>
       <c r="D366" t="s">
-        <v>691</v>
+        <v>671</v>
       </c>
       <c r="E366" t="s">
         <v>108</v>
       </c>
       <c r="F366">
-        <v>200</v>
+        <v>1</v>
       </c>
     </row>
     <row r="367" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A367">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="B367" s="15" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
       <c r="C367" t="s">
-        <v>603</v>
+        <v>202</v>
       </c>
       <c r="D367" t="s">
-        <v>692</v>
+        <v>181</v>
       </c>
       <c r="E367" t="s">
-        <v>528</v>
-      </c>
-      <c r="F367"/>
-    </row>
-    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A368">
-        <v>68</v>
-      </c>
-      <c r="B368" s="15" t="s">
-        <v>714</v>
-      </c>
-      <c r="C368" t="s">
-        <v>693</v>
-      </c>
-      <c r="D368" t="s">
-        <v>694</v>
-      </c>
-      <c r="E368" t="s">
-        <v>108</v>
-      </c>
-      <c r="F368">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="369" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A369">
-        <v>69</v>
-      </c>
-      <c r="B369" s="15" t="s">
-        <v>714</v>
-      </c>
-      <c r="C369" t="s">
-        <v>695</v>
-      </c>
-      <c r="D369" t="s">
-        <v>696</v>
-      </c>
-      <c r="E369" t="s">
-        <v>528</v>
-      </c>
-      <c r="F369"/>
-    </row>
-    <row r="370" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A370">
-        <v>70</v>
-      </c>
-      <c r="B370" s="15" t="s">
-        <v>714</v>
-      </c>
-      <c r="C370" t="s">
-        <v>372</v>
-      </c>
-      <c r="D370" t="s">
-        <v>560</v>
-      </c>
-      <c r="E370" t="s">
-        <v>544</v>
-      </c>
-      <c r="F370"/>
-    </row>
-    <row r="371" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A371">
-        <v>71</v>
-      </c>
-      <c r="B371" s="15" t="s">
-        <v>714</v>
-      </c>
-      <c r="C371" t="s">
-        <v>374</v>
-      </c>
-      <c r="D371" t="s">
-        <v>561</v>
-      </c>
-      <c r="E371" t="s">
-        <v>544</v>
-      </c>
-      <c r="F371"/>
-    </row>
-    <row r="372" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A372">
-        <v>72</v>
-      </c>
-      <c r="B372" s="15" t="s">
-        <v>714</v>
-      </c>
-      <c r="C372" t="s">
-        <v>376</v>
-      </c>
-      <c r="D372" t="s">
-        <v>697</v>
-      </c>
-      <c r="E372" t="s">
-        <v>544</v>
-      </c>
-      <c r="F372"/>
-    </row>
-    <row r="373" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A373">
-        <v>73</v>
-      </c>
-      <c r="B373" s="15" t="s">
-        <v>714</v>
-      </c>
-      <c r="C373" t="s">
-        <v>698</v>
-      </c>
-      <c r="D373" t="s">
-        <v>699</v>
-      </c>
-      <c r="E373" t="s">
-        <v>544</v>
-      </c>
-      <c r="F373"/>
-    </row>
-    <row r="374" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A374">
-        <v>74</v>
-      </c>
-      <c r="B374" s="15" t="s">
-        <v>714</v>
-      </c>
-      <c r="C374" t="s">
-        <v>494</v>
-      </c>
-      <c r="D374" t="s">
-        <v>700</v>
-      </c>
-      <c r="E374" t="s">
-        <v>544</v>
-      </c>
-      <c r="F374"/>
-    </row>
-    <row r="375" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A375">
-        <v>75</v>
-      </c>
-      <c r="B375" s="15" t="s">
-        <v>714</v>
-      </c>
-      <c r="C375" t="s">
-        <v>496</v>
-      </c>
-      <c r="D375" t="s">
-        <v>565</v>
-      </c>
-      <c r="E375" t="s">
-        <v>544</v>
-      </c>
-      <c r="F375"/>
-    </row>
-    <row r="376" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A376">
-        <v>76</v>
-      </c>
-      <c r="B376" s="15" t="s">
-        <v>714</v>
-      </c>
-      <c r="C376" t="s">
-        <v>498</v>
-      </c>
-      <c r="D376" t="s">
-        <v>701</v>
-      </c>
-      <c r="E376" t="s">
-        <v>544</v>
-      </c>
-      <c r="F376"/>
-    </row>
-    <row r="377" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A377">
-        <v>77</v>
-      </c>
-      <c r="B377" s="15" t="s">
-        <v>714</v>
-      </c>
-      <c r="C377" t="s">
-        <v>504</v>
-      </c>
-      <c r="D377" t="s">
-        <v>702</v>
-      </c>
-      <c r="E377" t="s">
-        <v>544</v>
-      </c>
-      <c r="F377"/>
-    </row>
-    <row r="378" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A378">
-        <v>78</v>
-      </c>
-      <c r="B378" s="15" t="s">
-        <v>714</v>
-      </c>
-      <c r="C378" t="s">
-        <v>502</v>
-      </c>
-      <c r="D378" t="s">
-        <v>703</v>
-      </c>
-      <c r="E378" t="s">
-        <v>544</v>
-      </c>
-      <c r="F378"/>
-    </row>
-    <row r="379" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A379">
-        <v>79</v>
-      </c>
-      <c r="B379" s="15" t="s">
-        <v>714</v>
-      </c>
-      <c r="C379" t="s">
-        <v>500</v>
-      </c>
-      <c r="D379" t="s">
-        <v>569</v>
-      </c>
-      <c r="E379" t="s">
-        <v>544</v>
-      </c>
-      <c r="F379"/>
-    </row>
-    <row r="380" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A380">
-        <v>80</v>
-      </c>
-      <c r="B380" s="15" t="s">
-        <v>714</v>
-      </c>
-      <c r="C380" t="s">
-        <v>704</v>
-      </c>
-      <c r="D380" t="s">
-        <v>705</v>
-      </c>
-      <c r="E380" t="s">
-        <v>528</v>
-      </c>
-      <c r="F380"/>
-    </row>
-    <row r="381" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A381">
-        <v>81</v>
-      </c>
-      <c r="B381" s="15" t="s">
-        <v>714</v>
-      </c>
-      <c r="C381" t="s">
-        <v>617</v>
-      </c>
-      <c r="D381" t="s">
-        <v>618</v>
-      </c>
-      <c r="E381" t="s">
-        <v>544</v>
-      </c>
-      <c r="F381"/>
-    </row>
-    <row r="382" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A382">
-        <v>82</v>
-      </c>
-      <c r="B382" s="15" t="s">
-        <v>714</v>
-      </c>
-      <c r="C382" t="s">
-        <v>706</v>
-      </c>
-      <c r="D382" t="s">
-        <v>707</v>
-      </c>
-      <c r="E382" t="s">
-        <v>108</v>
-      </c>
-      <c r="F382">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="383" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A383">
-        <v>83</v>
-      </c>
-      <c r="B383" s="15" t="s">
-        <v>714</v>
-      </c>
-      <c r="C383" t="s">
-        <v>219</v>
-      </c>
-      <c r="D383" t="s">
-        <v>220</v>
-      </c>
-      <c r="E383" t="s">
-        <v>655</v>
-      </c>
-      <c r="F383"/>
-    </row>
-    <row r="384" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A384">
-        <v>84</v>
-      </c>
-      <c r="B384" s="15" t="s">
-        <v>714</v>
-      </c>
-      <c r="C384" t="s">
-        <v>221</v>
-      </c>
-      <c r="D384" t="s">
-        <v>222</v>
-      </c>
-      <c r="E384" t="s">
-        <v>655</v>
-      </c>
-      <c r="F384"/>
-    </row>
-    <row r="385" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A385">
-        <v>85</v>
-      </c>
-      <c r="B385" s="15" t="s">
-        <v>714</v>
-      </c>
-      <c r="C385" t="s">
-        <v>230</v>
-      </c>
-      <c r="D385" t="s">
-        <v>577</v>
-      </c>
-      <c r="E385" t="s">
-        <v>528</v>
-      </c>
-      <c r="F385"/>
-    </row>
-    <row r="386" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A386">
-        <v>86</v>
-      </c>
-      <c r="B386" s="15" t="s">
-        <v>714</v>
-      </c>
-      <c r="C386" t="s">
-        <v>328</v>
-      </c>
-      <c r="D386" t="s">
-        <v>708</v>
-      </c>
-      <c r="E386" t="s">
-        <v>108</v>
-      </c>
-      <c r="F386">
+        <v>108</v>
+      </c>
+      <c r="F367">
         <v>1</v>
       </c>
     </row>
-    <row r="387" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A387">
-        <v>87</v>
-      </c>
-      <c r="B387" s="15" t="s">
-        <v>714</v>
-      </c>
-      <c r="C387" t="s">
-        <v>326</v>
-      </c>
-      <c r="D387" t="s">
-        <v>709</v>
-      </c>
-      <c r="E387" t="s">
-        <v>108</v>
-      </c>
-      <c r="F387">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="388" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A388">
-        <v>88</v>
-      </c>
-      <c r="B388" s="15" t="s">
-        <v>714</v>
-      </c>
-      <c r="C388" t="s">
-        <v>202</v>
-      </c>
-      <c r="D388" t="s">
-        <v>181</v>
-      </c>
-      <c r="E388" t="s">
-        <v>108</v>
-      </c>
-      <c r="F388">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="389" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A389">
-        <v>89</v>
-      </c>
-      <c r="B389" s="15" t="s">
-        <v>714</v>
-      </c>
-      <c r="C389" t="s">
-        <v>710</v>
-      </c>
-      <c r="D389" t="s">
-        <v>711</v>
-      </c>
-      <c r="E389" t="s">
-        <v>108</v>
-      </c>
-      <c r="F389">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="390" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A390">
-        <v>90</v>
-      </c>
-      <c r="B390" s="15" t="s">
-        <v>714</v>
-      </c>
-      <c r="C390" t="s">
-        <v>712</v>
-      </c>
-      <c r="D390" t="s">
-        <v>713</v>
-      </c>
-      <c r="E390" t="s">
-        <v>108</v>
-      </c>
-      <c r="F390">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:P300" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
+  <autoFilter ref="A1:P367" xr:uid="{00000000-0009-0000-0000-000002000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="ADES"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>

</xml_diff>

<commit_message>
Filter safety data add NFRLT
</commit_message>
<xml_diff>
--- a/specifications/er_spec.xlsx
+++ b/specifications/er_spec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff.dickinson\Documents\GitHub\er-standards\specifications\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60688A8A-3088-4869-939B-7297522B42FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D23FCC6-3DA2-4D85-B99A-F141DF4115D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Documents!$A$1:$C$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Methods!$A$1:$H$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ValueLevel!$A$1:$P$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$1:$P$367</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$1:$P$430</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">WhereClauses!$A$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2390" uniqueCount="687">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2398" uniqueCount="687">
   <si>
     <t>Attribute</t>
   </si>
@@ -2975,13 +2975,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:P429"/>
+  <dimension ref="A1:P431"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D406" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D387" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H420" sqref="H420"/>
+      <selection pane="bottomRight" activeCell="M392" sqref="M392"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3054,7 +3054,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3077,7 +3077,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="3" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3100,7 +3100,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3123,7 +3123,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3169,7 +3169,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="8" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3215,7 +3215,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="9" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3238,7 +3238,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3264,7 +3264,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="11" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3290,7 +3290,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="12" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3313,7 +3313,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3333,7 +3333,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3362,7 +3362,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3388,7 +3388,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3414,7 +3414,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3440,7 +3440,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="1:15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3492,7 +3492,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3518,7 +3518,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="21" spans="1:15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3544,7 +3544,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="22" spans="1:15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3567,7 +3567,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3590,7 +3590,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="24" spans="1:15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3613,7 +3613,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="25" spans="1:15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3636,7 +3636,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="26" spans="1:15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3659,7 +3659,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="27" spans="1:15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3682,7 +3682,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="28" spans="1:15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3705,7 +3705,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="29" spans="1:15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3728,7 +3728,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="30" spans="1:15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3754,7 +3754,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="31" spans="1:15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3780,7 +3780,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="32" spans="1:15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3800,7 +3800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3820,7 +3820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3846,7 +3846,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="35" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3872,7 +3872,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="36" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3895,7 +3895,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="37" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3918,7 +3918,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="38" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3941,7 +3941,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="39" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3961,7 +3961,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3984,7 +3984,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="41" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4007,7 +4007,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="42" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4027,7 +4027,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4053,7 +4053,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="44" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4073,7 +4073,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="45" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4093,7 +4093,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="46" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4113,7 +4113,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="47" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4133,7 +4133,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="48" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4156,7 +4156,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="49" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4179,7 +4179,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="50" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4205,7 +4205,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="51" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4228,7 +4228,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="52" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4251,7 +4251,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="53" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4274,7 +4274,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="54" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4294,7 +4294,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4314,7 +4314,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4334,7 +4334,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4354,7 +4354,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4374,7 +4374,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4394,7 +4394,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4414,7 +4414,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4434,7 +4434,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4454,7 +4454,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4474,7 +4474,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4494,7 +4494,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="65" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4517,7 +4517,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="66" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4540,7 +4540,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="67" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4563,7 +4563,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="68" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4586,7 +4586,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="69" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4609,7 +4609,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="70" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4632,7 +4632,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="71" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4652,7 +4652,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="72" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4672,7 +4672,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4692,7 +4692,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4712,7 +4712,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="75" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4732,7 +4732,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="76" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -4755,7 +4755,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="77" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -4778,7 +4778,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="78" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -4798,7 +4798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -4821,7 +4821,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="80" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -4841,7 +4841,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -4861,7 +4861,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="82" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -4881,7 +4881,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="83" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -4901,7 +4901,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="84" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -4921,7 +4921,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -4941,7 +4941,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -4961,7 +4961,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -4981,7 +4981,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="88" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -5001,7 +5001,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="89" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -5021,7 +5021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -5041,7 +5041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -5061,7 +5061,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="92" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -5081,7 +5081,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="93" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -5101,7 +5101,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="94" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="95" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -5141,7 +5141,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="96" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -5161,7 +5161,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="97" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -5181,7 +5181,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="98" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -5201,7 +5201,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="99" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -5221,7 +5221,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="100" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -5241,7 +5241,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="101" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -5261,7 +5261,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="102" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -5281,7 +5281,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="103" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -5301,7 +5301,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="104" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -5321,7 +5321,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="105" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -5341,7 +5341,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="106" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -5361,7 +5361,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="107" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -5381,7 +5381,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="108" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -5404,7 +5404,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="109" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -5427,7 +5427,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="110" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -5450,7 +5450,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="111" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -5473,7 +5473,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="112" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -5496,7 +5496,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="113" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -5519,7 +5519,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="114" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -5539,7 +5539,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="115" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -5559,7 +5559,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="116" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -5579,7 +5579,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="117" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -5599,7 +5599,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="118" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -5619,7 +5619,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="119" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -5639,7 +5639,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="120" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -5659,7 +5659,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="121" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -5679,7 +5679,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="122" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -5699,7 +5699,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="123" spans="1:16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
@@ -9736,7 +9736,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>1</v>
       </c>
@@ -9756,7 +9756,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>2</v>
       </c>
@@ -9774,7 +9774,7 @@
       </c>
       <c r="F302"/>
     </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>3</v>
       </c>
@@ -9794,7 +9794,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>4</v>
       </c>
@@ -9812,7 +9812,7 @@
       </c>
       <c r="F304"/>
     </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>5</v>
       </c>
@@ -9832,7 +9832,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>6</v>
       </c>
@@ -9850,7 +9850,7 @@
       </c>
       <c r="F306"/>
     </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>7</v>
       </c>
@@ -9870,7 +9870,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>8</v>
       </c>
@@ -9888,7 +9888,7 @@
       </c>
       <c r="F308"/>
     </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>9</v>
       </c>
@@ -9906,7 +9906,7 @@
       </c>
       <c r="F309"/>
     </row>
-    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>10</v>
       </c>
@@ -9926,7 +9926,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>11</v>
       </c>
@@ -9944,7 +9944,7 @@
       </c>
       <c r="F311"/>
     </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>12</v>
       </c>
@@ -9964,7 +9964,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>13</v>
       </c>
@@ -9984,7 +9984,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>14</v>
       </c>
@@ -10002,7 +10002,7 @@
       </c>
       <c r="F314"/>
     </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>15</v>
       </c>
@@ -10022,7 +10022,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>16</v>
       </c>
@@ -10040,7 +10040,7 @@
       </c>
       <c r="F316"/>
     </row>
-    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>18</v>
       </c>
@@ -10058,7 +10058,7 @@
       </c>
       <c r="F317"/>
     </row>
-    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>19</v>
       </c>
@@ -10078,7 +10078,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>20</v>
       </c>
@@ -10096,7 +10096,7 @@
       </c>
       <c r="F319"/>
     </row>
-    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>21</v>
       </c>
@@ -10116,7 +10116,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>22</v>
       </c>
@@ -10134,7 +10134,7 @@
       </c>
       <c r="F321"/>
     </row>
-    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>23</v>
       </c>
@@ -10154,7 +10154,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>24</v>
       </c>
@@ -10172,7 +10172,7 @@
       </c>
       <c r="F323"/>
     </row>
-    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>25</v>
       </c>
@@ -10192,7 +10192,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>26</v>
       </c>
@@ -10210,7 +10210,7 @@
       </c>
       <c r="F325"/>
     </row>
-    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>27</v>
       </c>
@@ -10230,7 +10230,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>28</v>
       </c>
@@ -10250,7 +10250,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>29</v>
       </c>
@@ -10268,7 +10268,7 @@
       </c>
       <c r="F328"/>
     </row>
-    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>30</v>
       </c>
@@ -10286,7 +10286,7 @@
       </c>
       <c r="F329"/>
     </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>31</v>
       </c>
@@ -10306,7 +10306,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>32</v>
       </c>
@@ -10324,7 +10324,7 @@
       </c>
       <c r="F331"/>
     </row>
-    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>33</v>
       </c>
@@ -10344,7 +10344,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>34</v>
       </c>
@@ -10364,7 +10364,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>35</v>
       </c>
@@ -10384,7 +10384,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>36</v>
       </c>
@@ -10404,7 +10404,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>37</v>
       </c>
@@ -10422,7 +10422,7 @@
       </c>
       <c r="F336"/>
     </row>
-    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>38</v>
       </c>
@@ -10442,7 +10442,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>39</v>
       </c>
@@ -10460,7 +10460,7 @@
       </c>
       <c r="F338"/>
     </row>
-    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>40</v>
       </c>
@@ -10480,7 +10480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>41</v>
       </c>
@@ -10500,7 +10500,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>42</v>
       </c>
@@ -10520,7 +10520,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>43</v>
       </c>
@@ -10538,7 +10538,7 @@
       </c>
       <c r="F342"/>
     </row>
-    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>44</v>
       </c>
@@ -10556,7 +10556,7 @@
       </c>
       <c r="F343"/>
     </row>
-    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>45</v>
       </c>
@@ -10574,7 +10574,7 @@
       </c>
       <c r="F344"/>
     </row>
-    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>46</v>
       </c>
@@ -10592,7 +10592,7 @@
       </c>
       <c r="F345"/>
     </row>
-    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>47</v>
       </c>
@@ -10610,7 +10610,7 @@
       </c>
       <c r="F346"/>
     </row>
-    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>48</v>
       </c>
@@ -10630,7 +10630,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>49</v>
       </c>
@@ -10650,7 +10650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349">
         <v>51</v>
       </c>
@@ -10668,7 +10668,7 @@
       </c>
       <c r="F349"/>
     </row>
-    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350">
         <v>52</v>
       </c>
@@ -10686,7 +10686,7 @@
       </c>
       <c r="F350"/>
     </row>
-    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>70</v>
       </c>
@@ -10704,7 +10704,7 @@
       </c>
       <c r="F351"/>
     </row>
-    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352">
         <v>71</v>
       </c>
@@ -10722,7 +10722,7 @@
       </c>
       <c r="F352"/>
     </row>
-    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A353">
         <v>72</v>
       </c>
@@ -10740,7 +10740,7 @@
       </c>
       <c r="F353"/>
     </row>
-    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354">
         <v>73</v>
       </c>
@@ -10758,7 +10758,7 @@
       </c>
       <c r="F354"/>
     </row>
-    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355">
         <v>74</v>
       </c>
@@ -10776,7 +10776,7 @@
       </c>
       <c r="F355"/>
     </row>
-    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356">
         <v>75</v>
       </c>
@@ -10794,7 +10794,7 @@
       </c>
       <c r="F356"/>
     </row>
-    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357">
         <v>76</v>
       </c>
@@ -10812,7 +10812,7 @@
       </c>
       <c r="F357"/>
     </row>
-    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358">
         <v>77</v>
       </c>
@@ -10830,7 +10830,7 @@
       </c>
       <c r="F358"/>
     </row>
-    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359">
         <v>78</v>
       </c>
@@ -10848,7 +10848,7 @@
       </c>
       <c r="F359"/>
     </row>
-    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360">
         <v>79</v>
       </c>
@@ -10866,7 +10866,7 @@
       </c>
       <c r="F360"/>
     </row>
-    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361">
         <v>81</v>
       </c>
@@ -10884,7 +10884,7 @@
       </c>
       <c r="F361"/>
     </row>
-    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362">
         <v>83</v>
       </c>
@@ -10902,7 +10902,7 @@
       </c>
       <c r="F362"/>
     </row>
-    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363">
         <v>84</v>
       </c>
@@ -10920,7 +10920,7 @@
       </c>
       <c r="F363"/>
     </row>
-    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364">
         <v>85</v>
       </c>
@@ -10938,7 +10938,7 @@
       </c>
       <c r="F364"/>
     </row>
-    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365">
         <v>86</v>
       </c>
@@ -10958,7 +10958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366">
         <v>87</v>
       </c>
@@ -10978,7 +10978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A367">
         <v>88</v>
       </c>
@@ -11287,7 +11287,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="385" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A385">
         <v>19</v>
       </c>
@@ -11304,7 +11304,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="386" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A386">
         <v>20</v>
       </c>
@@ -11321,7 +11321,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="387" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A387">
         <v>21</v>
       </c>
@@ -11338,7 +11338,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="388" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A388">
         <v>22</v>
       </c>
@@ -11355,7 +11355,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="389" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A389">
         <v>23</v>
       </c>
@@ -11372,7 +11372,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="390" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A390">
         <v>24</v>
       </c>
@@ -11389,7 +11389,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="391" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A391">
         <v>25</v>
       </c>
@@ -11406,7 +11406,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="392" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A392">
         <v>26</v>
       </c>
@@ -11423,7 +11423,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="393" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A393">
         <v>27</v>
       </c>
@@ -11440,7 +11440,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="394" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A394">
         <v>28</v>
       </c>
@@ -11457,7 +11457,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="395" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A395">
         <v>29</v>
       </c>
@@ -11474,7 +11474,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="396" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A396">
         <v>30</v>
       </c>
@@ -11482,129 +11482,135 @@
         <v>685</v>
       </c>
       <c r="C396" t="s">
-        <v>292</v>
+        <v>258</v>
       </c>
       <c r="D396" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
       <c r="E396" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="397" spans="1:5" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+      <c r="F396">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="397" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A397">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B397" s="15" t="s">
         <v>685</v>
       </c>
       <c r="C397" t="s">
-        <v>290</v>
+        <v>270</v>
       </c>
       <c r="D397" t="s">
-        <v>291</v>
+        <v>271</v>
       </c>
       <c r="E397" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="398" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F397">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="398" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A398">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B398" s="15" t="s">
         <v>685</v>
       </c>
       <c r="C398" t="s">
-        <v>312</v>
+        <v>292</v>
       </c>
       <c r="D398" t="s">
-        <v>313</v>
+        <v>293</v>
       </c>
       <c r="E398" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="399" spans="1:5" x14ac:dyDescent="0.25">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="399" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A399">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B399" s="15" t="s">
         <v>685</v>
       </c>
       <c r="C399" t="s">
-        <v>630</v>
+        <v>290</v>
       </c>
       <c r="D399" t="s">
-        <v>631</v>
+        <v>291</v>
       </c>
       <c r="E399" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="400" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A400">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B400" s="15" t="s">
         <v>685</v>
       </c>
       <c r="C400" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D400" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E400" t="s">
-        <v>108</v>
+        <v>544</v>
       </c>
     </row>
     <row r="401" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A401">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B401" s="15" t="s">
         <v>685</v>
       </c>
       <c r="C401" t="s">
-        <v>318</v>
+        <v>630</v>
       </c>
       <c r="D401" t="s">
-        <v>319</v>
+        <v>631</v>
       </c>
       <c r="E401" t="s">
-        <v>544</v>
+        <v>108</v>
       </c>
     </row>
     <row r="402" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A402">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B402" s="15" t="s">
         <v>685</v>
       </c>
       <c r="C402" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="D402" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="E402" t="s">
-        <v>544</v>
+        <v>108</v>
       </c>
     </row>
     <row r="403" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A403">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B403" s="15" t="s">
         <v>685</v>
       </c>
       <c r="C403" t="s">
-        <v>675</v>
+        <v>318</v>
       </c>
       <c r="D403" t="s">
-        <v>676</v>
+        <v>319</v>
       </c>
       <c r="E403" t="s">
         <v>544</v>
@@ -11612,16 +11618,16 @@
     </row>
     <row r="404" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A404">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B404" s="15" t="s">
         <v>685</v>
       </c>
       <c r="C404" t="s">
-        <v>677</v>
+        <v>320</v>
       </c>
       <c r="D404" t="s">
-        <v>678</v>
+        <v>321</v>
       </c>
       <c r="E404" t="s">
         <v>544</v>
@@ -11629,16 +11635,16 @@
     </row>
     <row r="405" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A405">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B405" s="15" t="s">
         <v>685</v>
       </c>
       <c r="C405" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="D405" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="E405" t="s">
         <v>544</v>
@@ -11646,50 +11652,50 @@
     </row>
     <row r="406" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A406">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B406" s="15" t="s">
         <v>685</v>
       </c>
       <c r="C406" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="D406" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="E406" t="s">
-        <v>528</v>
+        <v>544</v>
       </c>
     </row>
     <row r="407" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A407">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B407" s="15" t="s">
         <v>685</v>
       </c>
       <c r="C407" t="s">
-        <v>300</v>
+        <v>679</v>
       </c>
       <c r="D407" t="s">
-        <v>301</v>
+        <v>680</v>
       </c>
       <c r="E407" t="s">
-        <v>654</v>
+        <v>544</v>
       </c>
     </row>
     <row r="408" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A408">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B408" s="15" t="s">
         <v>685</v>
       </c>
       <c r="C408" t="s">
-        <v>308</v>
+        <v>681</v>
       </c>
       <c r="D408" t="s">
-        <v>309</v>
+        <v>682</v>
       </c>
       <c r="E408" t="s">
         <v>528</v>
@@ -11697,67 +11703,67 @@
     </row>
     <row r="409" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A409">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B409" s="15" t="s">
         <v>685</v>
       </c>
       <c r="C409" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="D409" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="E409" t="s">
-        <v>108</v>
+        <v>654</v>
       </c>
     </row>
     <row r="410" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A410">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B410" s="15" t="s">
         <v>685</v>
       </c>
       <c r="C410" t="s">
-        <v>593</v>
+        <v>308</v>
       </c>
       <c r="D410" t="s">
-        <v>665</v>
+        <v>309</v>
       </c>
       <c r="E410" t="s">
-        <v>544</v>
+        <v>528</v>
       </c>
     </row>
     <row r="411" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A411">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B411" s="15" t="s">
         <v>685</v>
       </c>
       <c r="C411" t="s">
-        <v>609</v>
+        <v>316</v>
       </c>
       <c r="D411" t="s">
-        <v>666</v>
+        <v>317</v>
       </c>
       <c r="E411" t="s">
-        <v>544</v>
+        <v>108</v>
       </c>
     </row>
     <row r="412" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A412">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="B412" s="15" t="s">
         <v>685</v>
       </c>
       <c r="C412" t="s">
-        <v>372</v>
+        <v>593</v>
       </c>
       <c r="D412" t="s">
-        <v>560</v>
+        <v>665</v>
       </c>
       <c r="E412" t="s">
         <v>544</v>
@@ -11765,16 +11771,16 @@
     </row>
     <row r="413" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A413">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="B413" s="15" t="s">
         <v>685</v>
       </c>
       <c r="C413" t="s">
-        <v>374</v>
+        <v>609</v>
       </c>
       <c r="D413" t="s">
-        <v>561</v>
+        <v>666</v>
       </c>
       <c r="E413" t="s">
         <v>544</v>
@@ -11782,16 +11788,16 @@
     </row>
     <row r="414" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A414">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B414" s="15" t="s">
         <v>685</v>
       </c>
       <c r="C414" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="D414" t="s">
-        <v>667</v>
+        <v>560</v>
       </c>
       <c r="E414" t="s">
         <v>544</v>
@@ -11799,16 +11805,16 @@
     </row>
     <row r="415" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A415">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B415" s="15" t="s">
         <v>685</v>
       </c>
       <c r="C415" t="s">
-        <v>477</v>
+        <v>374</v>
       </c>
       <c r="D415" t="s">
-        <v>674</v>
+        <v>561</v>
       </c>
       <c r="E415" t="s">
         <v>544</v>
@@ -11816,16 +11822,16 @@
     </row>
     <row r="416" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A416">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B416" s="15" t="s">
         <v>685</v>
       </c>
       <c r="C416" t="s">
-        <v>494</v>
+        <v>376</v>
       </c>
       <c r="D416" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="E416" t="s">
         <v>544</v>
@@ -11833,16 +11839,16 @@
     </row>
     <row r="417" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A417">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B417" s="15" t="s">
         <v>685</v>
       </c>
       <c r="C417" t="s">
-        <v>496</v>
+        <v>477</v>
       </c>
       <c r="D417" t="s">
-        <v>565</v>
+        <v>674</v>
       </c>
       <c r="E417" t="s">
         <v>544</v>
@@ -11850,16 +11856,16 @@
     </row>
     <row r="418" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A418">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B418" s="15" t="s">
         <v>685</v>
       </c>
       <c r="C418" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="D418" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="E418" t="s">
         <v>544</v>
@@ -11867,16 +11873,16 @@
     </row>
     <row r="419" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A419">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B419" s="15" t="s">
         <v>685</v>
       </c>
       <c r="C419" t="s">
-        <v>504</v>
-      </c>
-      <c r="D419" s="15" t="s">
-        <v>567</v>
+        <v>496</v>
+      </c>
+      <c r="D419" t="s">
+        <v>565</v>
       </c>
       <c r="E419" t="s">
         <v>544</v>
@@ -11884,16 +11890,16 @@
     </row>
     <row r="420" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A420">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B420" s="15" t="s">
         <v>685</v>
       </c>
       <c r="C420" t="s">
-        <v>502</v>
-      </c>
-      <c r="D420" s="15" t="s">
-        <v>568</v>
+        <v>498</v>
+      </c>
+      <c r="D420" t="s">
+        <v>669</v>
       </c>
       <c r="E420" t="s">
         <v>544</v>
@@ -11901,16 +11907,16 @@
     </row>
     <row r="421" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A421">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B421" s="15" t="s">
         <v>685</v>
       </c>
       <c r="C421" t="s">
-        <v>500</v>
-      </c>
-      <c r="D421" t="s">
-        <v>569</v>
+        <v>504</v>
+      </c>
+      <c r="D421" s="15" t="s">
+        <v>567</v>
       </c>
       <c r="E421" t="s">
         <v>544</v>
@@ -11918,16 +11924,16 @@
     </row>
     <row r="422" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A422">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B422" s="15" t="s">
         <v>685</v>
       </c>
       <c r="C422" t="s">
-        <v>617</v>
-      </c>
-      <c r="D422" t="s">
-        <v>618</v>
+        <v>502</v>
+      </c>
+      <c r="D422" s="15" t="s">
+        <v>568</v>
       </c>
       <c r="E422" t="s">
         <v>544</v>
@@ -11935,101 +11941,101 @@
     </row>
     <row r="423" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A423">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B423" s="15" t="s">
         <v>685</v>
       </c>
       <c r="C423" t="s">
-        <v>219</v>
+        <v>500</v>
       </c>
       <c r="D423" t="s">
-        <v>220</v>
+        <v>569</v>
       </c>
       <c r="E423" t="s">
-        <v>654</v>
+        <v>544</v>
       </c>
     </row>
     <row r="424" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A424">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B424" s="15" t="s">
         <v>685</v>
       </c>
       <c r="C424" t="s">
-        <v>221</v>
+        <v>617</v>
       </c>
       <c r="D424" t="s">
-        <v>222</v>
+        <v>618</v>
       </c>
       <c r="E424" t="s">
-        <v>654</v>
+        <v>544</v>
       </c>
     </row>
     <row r="425" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A425">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B425" s="15" t="s">
         <v>685</v>
       </c>
       <c r="C425" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="D425" t="s">
-        <v>577</v>
+        <v>220</v>
       </c>
       <c r="E425" t="s">
-        <v>528</v>
+        <v>654</v>
       </c>
     </row>
     <row r="426" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A426">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B426" s="15" t="s">
         <v>685</v>
       </c>
       <c r="C426" t="s">
-        <v>328</v>
+        <v>221</v>
       </c>
       <c r="D426" t="s">
-        <v>670</v>
+        <v>222</v>
       </c>
       <c r="E426" t="s">
-        <v>108</v>
+        <v>654</v>
       </c>
     </row>
     <row r="427" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A427">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B427" s="15" t="s">
         <v>685</v>
       </c>
       <c r="C427" t="s">
-        <v>326</v>
+        <v>230</v>
       </c>
       <c r="D427" t="s">
-        <v>683</v>
+        <v>577</v>
       </c>
       <c r="E427" t="s">
-        <v>108</v>
+        <v>528</v>
       </c>
     </row>
     <row r="428" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A428">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B428" s="15" t="s">
         <v>685</v>
       </c>
       <c r="C428" t="s">
-        <v>619</v>
+        <v>328</v>
       </c>
       <c r="D428" t="s">
-        <v>684</v>
+        <v>670</v>
       </c>
       <c r="E428" t="s">
         <v>108</v>
@@ -12037,26 +12043,61 @@
     </row>
     <row r="429" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A429">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B429" s="15" t="s">
         <v>685</v>
       </c>
       <c r="C429" t="s">
+        <v>326</v>
+      </c>
+      <c r="D429" t="s">
+        <v>683</v>
+      </c>
+      <c r="E429" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="430" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A430">
+        <v>83</v>
+      </c>
+      <c r="B430" s="15" t="s">
+        <v>685</v>
+      </c>
+      <c r="C430" t="s">
+        <v>619</v>
+      </c>
+      <c r="D430" t="s">
+        <v>684</v>
+      </c>
+      <c r="E430" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="431" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A431">
+        <v>84</v>
+      </c>
+      <c r="B431" s="15" t="s">
+        <v>685</v>
+      </c>
+      <c r="C431" t="s">
         <v>202</v>
       </c>
-      <c r="D429" t="s">
+      <c r="D431" t="s">
         <v>181</v>
       </c>
-      <c r="E429" t="s">
+      <c r="E431" t="s">
         <v>108</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P367" xr:uid="{00000000-0009-0000-0000-000002000000}">
+  <autoFilter ref="A1:P430" xr:uid="{00000000-0009-0000-0000-000002000000}">
     <filterColumn colId="1">
       <filters>
-        <filter val="ADES"/>
+        <filter val="ADPC"/>
+        <filter val="ADTRR"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>